<commit_message>
Adiciona resolução das questoes 1, 2, 3, 4, 7
</commit_message>
<xml_diff>
--- a/series.xlsx
+++ b/series.xlsx
@@ -327,10 +327,10 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.86"/>
@@ -811,7 +811,7 @@
         <v>2019</v>
       </c>
       <c r="F21" s="8" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G21" s="8"/>
     </row>

</xml_diff>